<commit_message>
feat: update TalentTree config
更新天赋树表
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592AE4C6-6954-42FA-8AFB-C7873FE491F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A15586-CC39-40D1-9B38-CE09A3883E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,10 +726,6 @@
     <t>在无尽模式下，基地耐久提高{0}</t>
   </si>
   <si>
-    <t>1015|1016|1017|1018</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>距离增强</t>
   </si>
   <si>
@@ -770,10 +766,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>1039|1040|1041</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>1044|1045|1042|1043</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -868,6 +860,14 @@
   </si>
   <si>
     <t>未激活 icon 图标</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1016|1017|1018|1019</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1040|1041|1042</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1325,7 +1325,7 @@
         <v>12</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1366,7 +1366,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
@@ -1584,7 +1584,7 @@
         <v>1006</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>56</v>
@@ -1628,7 +1628,7 @@
         <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>62</v>
@@ -1967,8 +1967,8 @@
       <c r="F19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>230</v>
+      <c r="G19" s="7" t="s">
+        <v>273</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>105</v>
@@ -1997,7 +1997,7 @@
         <v>109</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>143</v>
@@ -2038,7 +2038,7 @@
         <v>110</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>144</v>
@@ -2079,7 +2079,7 @@
         <v>111</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>145</v>
@@ -2120,7 +2120,7 @@
         <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>146</v>
@@ -2161,7 +2161,7 @@
         <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>147</v>
@@ -2202,7 +2202,7 @@
         <v>114</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>148</v>
@@ -2243,7 +2243,7 @@
         <v>115</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>149</v>
@@ -2252,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G26" s="1">
         <v>1024</v>
@@ -2284,7 +2284,7 @@
         <v>116</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>150</v>
@@ -2325,7 +2325,7 @@
         <v>117</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>151</v>
@@ -2337,7 +2337,7 @@
         <v>178</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>105</v>
@@ -2366,7 +2366,7 @@
         <v>118</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>152</v>
@@ -2407,7 +2407,7 @@
         <v>119</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>153</v>
@@ -2448,7 +2448,7 @@
         <v>120</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>154</v>
@@ -2460,7 +2460,7 @@
         <v>1024</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>30</v>
@@ -2489,7 +2489,7 @@
         <v>121</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>155</v>
@@ -2501,7 +2501,7 @@
         <v>179</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>30</v>
@@ -2530,7 +2530,7 @@
         <v>122</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>156</v>
@@ -2571,7 +2571,7 @@
         <v>123</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>157</v>
@@ -2612,7 +2612,7 @@
         <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>158</v>
@@ -2653,7 +2653,7 @@
         <v>125</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>159</v>
@@ -2694,7 +2694,7 @@
         <v>126</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>160</v>
@@ -2735,7 +2735,7 @@
         <v>127</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>161</v>
@@ -2776,7 +2776,7 @@
         <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>162</v>
@@ -2817,7 +2817,7 @@
         <v>129</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>163</v>
@@ -2858,7 +2858,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>164</v>
@@ -2899,7 +2899,7 @@
         <v>131</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>165</v>
@@ -2940,7 +2940,7 @@
         <v>132</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>166</v>
@@ -2952,7 +2952,7 @@
         <v>181</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>105</v>
@@ -2981,7 +2981,7 @@
         <v>133</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>167</v>
@@ -3022,7 +3022,7 @@
         <v>134</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>168</v>
@@ -3063,7 +3063,7 @@
         <v>135</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>169</v>
@@ -3104,7 +3104,7 @@
         <v>136</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>170</v>
@@ -3145,7 +3145,7 @@
         <v>137</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>171</v>
@@ -3186,7 +3186,7 @@
         <v>138</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>172</v>
@@ -3227,7 +3227,7 @@
         <v>139</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>173</v>
@@ -3236,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>105</v>
@@ -3268,7 +3268,7 @@
         <v>140</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>174</v>
@@ -3306,7 +3306,7 @@
         <v>141</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>175</v>
@@ -3344,7 +3344,7 @@
         <v>142</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
feat: add talent max level
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\nevergiveup\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAF6144-8188-4FEA-94A6-6E7B573F97AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="278">
   <si>
     <t>int</t>
   </si>
@@ -69,9 +65,15 @@
     <t>cost</t>
   </si>
   <si>
+    <t>maxLevel</t>
+  </si>
+  <si>
     <t>icon</t>
   </si>
   <si>
+    <t>iconGray</t>
+  </si>
+  <si>
     <t>buffId</t>
   </si>
   <si>
@@ -81,6 +83,9 @@
     <t>descCN</t>
   </si>
   <si>
+    <t>TalentTreeid</t>
+  </si>
+  <si>
     <t>天赋名称</t>
   </si>
   <si>
@@ -102,9 +107,15 @@
     <t xml:space="preserve"> 解锁以及升级所需资源[[资源id,1级,2级,3级],[资源id,1级,2级,3级]]</t>
   </si>
   <si>
+    <t>最大等级</t>
+  </si>
+  <si>
     <t>icon 图标</t>
   </si>
   <si>
+    <t>未激活 icon 图标</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 天赋buff表的id</t>
   </si>
   <si>
@@ -156,6 +167,9 @@
     <t>talentItemCanvas_3</t>
   </si>
   <si>
+    <t>1005|1006</t>
+  </si>
+  <si>
     <t>1|10|20|40||2|10|20|40</t>
   </si>
   <si>
@@ -201,6 +215,9 @@
     <t>每个波次获得{0}能量</t>
   </si>
   <si>
+    <t>TalentTree_Name_6</t>
+  </si>
+  <si>
     <t>矿机升级</t>
   </si>
   <si>
@@ -219,6 +236,9 @@
     <t>TalentTree_Name_7</t>
   </si>
   <si>
+    <t>光元素增伤</t>
+  </si>
+  <si>
     <t>talentItemCanvas_7</t>
   </si>
   <si>
@@ -348,6 +368,9 @@
     <t>1011|1012|1013|1014</t>
   </si>
   <si>
+    <t>1016|1017|1018|1019</t>
+  </si>
+  <si>
     <t>1|10|20|40|65||2|10|20|40|65</t>
   </si>
   <si>
@@ -357,535 +380,500 @@
     <t>敌方受到伤害提高{0}%</t>
   </si>
   <si>
-    <t>TalentTreeid</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>TalentTree_Name_16</t>
   </si>
   <si>
+    <t>距离增强</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_16</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_16</t>
+  </si>
+  <si>
+    <t>攻击范围提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_17</t>
   </si>
   <si>
+    <t>物理斩杀</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_17</t>
+  </si>
+  <si>
+    <t>1|10||2|10</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_17</t>
+  </si>
+  <si>
+    <t>物理伤害对于血量低于20%的敌方造成伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_18</t>
   </si>
   <si>
+    <t>黯灭</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_18</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_18</t>
+  </si>
+  <si>
+    <t>敌方入场5秒内护甲减少{0}</t>
+  </si>
+  <si>
     <t>TalentTree_Name_19</t>
   </si>
   <si>
+    <t>希瓦</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_19</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_19</t>
+  </si>
+  <si>
+    <t>敌方入场5秒内魔抗减少{0}</t>
+  </si>
+  <si>
     <t>TalentTree_Name_20</t>
   </si>
   <si>
+    <t>高射火炮</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_20</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_20</t>
+  </si>
+  <si>
+    <t>对空中敌方造成伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_21</t>
   </si>
   <si>
+    <t>魔法压制</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_21</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_21</t>
+  </si>
+  <si>
+    <t>魔法伤害对于血量高于80%的敌方造成伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_22</t>
   </si>
   <si>
+    <t>元素压制</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_22</t>
+  </si>
+  <si>
+    <t>1020|1021</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_22</t>
+  </si>
+  <si>
+    <t>元素克制时造成伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_23</t>
   </si>
   <si>
+    <t>元素抵抗</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_23</t>
+  </si>
+  <si>
+    <t>1018|1019</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_23</t>
+  </si>
+  <si>
+    <t>元素被克制时的伤害减免减少{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_24</t>
   </si>
   <si>
+    <t>慧光2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_24</t>
+  </si>
+  <si>
+    <t>1022|1023</t>
+  </si>
+  <si>
+    <t>1025|1026|1027</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_24</t>
+  </si>
+  <si>
     <t>TalentTree_Name_25</t>
   </si>
   <si>
+    <t>物理精通</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_25</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_25</t>
+  </si>
+  <si>
     <t>TalentTree_Name_26</t>
   </si>
   <si>
+    <t>魔法升华</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_26</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_26</t>
+  </si>
+  <si>
     <t>TalentTree_Name_27</t>
   </si>
   <si>
+    <t>基地耐久2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_27</t>
+  </si>
+  <si>
+    <t>1029|1030</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_27</t>
+  </si>
+  <si>
     <t>TalentTree_Name_28</t>
   </si>
   <si>
+    <t>攻速增强2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_28</t>
+  </si>
+  <si>
+    <t>1025|1026</t>
+  </si>
+  <si>
+    <t>1031|1032|1033</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_28</t>
+  </si>
+  <si>
     <t>TalentTree_Name_29</t>
   </si>
   <si>
+    <t>天降能量2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_29</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_29</t>
+  </si>
+  <si>
     <t>TalentTree_Name_30</t>
   </si>
   <si>
+    <t>矿机升级2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_30</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_30</t>
+  </si>
+  <si>
     <t>TalentTree_Name_31</t>
   </si>
   <si>
+    <t>光元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_31</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_31</t>
+  </si>
+  <si>
     <t>TalentTree_Name_32</t>
   </si>
   <si>
+    <t>水元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_32</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_32</t>
+  </si>
+  <si>
     <t>TalentTree_Name_33</t>
   </si>
   <si>
+    <t>土元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_33</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_33</t>
+  </si>
+  <si>
     <t>TalentTree_Name_34</t>
   </si>
   <si>
+    <t>耐久恢复2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_34</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_34</t>
+  </si>
+  <si>
     <t>TalentTree_Name_35</t>
   </si>
   <si>
+    <t>暗元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_35</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_35</t>
+  </si>
+  <si>
     <t>TalentTree_Name_36</t>
   </si>
   <si>
+    <t>火元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_36</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_36</t>
+  </si>
+  <si>
     <t>TalentTree_Name_37</t>
   </si>
   <si>
+    <t>木元素增伤2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_37</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_37</t>
+  </si>
+  <si>
     <t>TalentTree_Name_38</t>
   </si>
   <si>
+    <t>敌方减速2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_38</t>
+  </si>
+  <si>
+    <t>1034|1030</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_38</t>
+  </si>
+  <si>
     <t>TalentTree_Name_39</t>
   </si>
   <si>
+    <t>慧光3</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_39</t>
+  </si>
+  <si>
+    <t>1035|1036|1037|1038</t>
+  </si>
+  <si>
+    <t>1040|1041|1042</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_39</t>
+  </si>
+  <si>
     <t>TalentTree_Name_40</t>
   </si>
   <si>
+    <t>距离增强2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_40</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_40</t>
+  </si>
+  <si>
     <t>TalentTree_Name_41</t>
   </si>
   <si>
+    <t>物理斩杀2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_41</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_41</t>
+  </si>
+  <si>
     <t>TalentTree_Name_42</t>
   </si>
   <si>
+    <t>黯灭2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_42</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_42</t>
+  </si>
+  <si>
     <t>TalentTree_Name_43</t>
   </si>
   <si>
+    <t>希瓦2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_43</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_43</t>
+  </si>
+  <si>
     <t>TalentTree_Name_44</t>
   </si>
   <si>
+    <t>高射火炮2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_44</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_44</t>
+  </si>
+  <si>
     <t>TalentTree_Name_45</t>
   </si>
   <si>
+    <t>魔法压制2</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_45</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_45</t>
+  </si>
+  <si>
     <t>TalentTree_Name_46</t>
   </si>
   <si>
+    <t>慧光4</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_46</t>
+  </si>
+  <si>
+    <t>1044|1045|1042|1043</t>
+  </si>
+  <si>
+    <t>1047|1048|1049</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_46</t>
+  </si>
+  <si>
     <t>TalentTree_Name_47</t>
   </si>
   <si>
+    <t>物理</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_47</t>
+  </si>
+  <si>
+    <t>1|100||2|100</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_47</t>
+  </si>
+  <si>
+    <t>在无尽模式下，物理伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_48</t>
   </si>
   <si>
+    <t>魔法</t>
+  </si>
+  <si>
+    <t>talentItemCanvas_48</t>
+  </si>
+  <si>
+    <t>TalentTree_Desc_48</t>
+  </si>
+  <si>
+    <t>在无尽模式下，魔法伤害提高{0}%</t>
+  </si>
+  <si>
     <t>TalentTree_Name_49</t>
   </si>
   <si>
-    <t>talentItemCanvas_16</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_17</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_18</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_19</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_20</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_21</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_22</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_23</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_24</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_25</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_26</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_27</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_28</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_29</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_30</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_31</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_32</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_33</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_34</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_35</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_36</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_37</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_38</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_39</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_40</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_41</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_42</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_43</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_44</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_45</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_46</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_47</t>
-  </si>
-  <si>
-    <t>talentItemCanvas_48</t>
+    <t>耐久</t>
   </si>
   <si>
     <t>talentItemCanvas_49</t>
   </si>
   <si>
-    <t>1018|1019</t>
-  </si>
-  <si>
-    <t>1022|1023</t>
-  </si>
-  <si>
-    <t>1025|1026</t>
-  </si>
-  <si>
-    <t>1034|1030</t>
-  </si>
-  <si>
-    <t>1035|1036|1037|1038</t>
-  </si>
-  <si>
-    <t>1005|1006</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1|10||2|10</t>
-  </si>
-  <si>
-    <t>1|100||2|100</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>TalentTree_Desc_16</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_17</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_18</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_19</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_20</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_21</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_22</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_23</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_24</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_25</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_26</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_27</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_28</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_29</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_30</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_31</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_32</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_33</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_34</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_35</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_36</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_37</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_38</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_39</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_40</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_41</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_42</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_43</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_44</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_45</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_46</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_47</t>
-  </si>
-  <si>
-    <t>TalentTree_Desc_48</t>
-  </si>
-  <si>
     <t>TalentTree_Desc_49</t>
   </si>
   <si>
-    <t>攻击范围提高{0}%</t>
-  </si>
-  <si>
-    <t>物理伤害对于血量低于20%的敌方造成伤害提高{0}%</t>
-  </si>
-  <si>
-    <t>敌方入场5秒内护甲减少{0}</t>
-  </si>
-  <si>
-    <t>敌方入场5秒内魔抗减少{0}</t>
-  </si>
-  <si>
-    <t>对空中敌方造成伤害提高{0}%</t>
-  </si>
-  <si>
-    <t>魔法伤害对于血量高于80%的敌方造成伤害提高{0}%</t>
-  </si>
-  <si>
-    <t>元素克制时造成伤害提高{0}%</t>
-  </si>
-  <si>
-    <t>元素被克制时的伤害减免减少{0}%</t>
-  </si>
-  <si>
-    <t>在无尽模式下，物理伤害提高{0}%</t>
-  </si>
-  <si>
-    <t>在无尽模式下，魔法伤害提高{0}%</t>
-  </si>
-  <si>
     <t>在无尽模式下，基地耐久提高{0}</t>
-  </si>
-  <si>
-    <t>距离增强</t>
-  </si>
-  <si>
-    <t>物理斩杀</t>
-  </si>
-  <si>
-    <t>黯灭</t>
-  </si>
-  <si>
-    <t>希瓦</t>
-  </si>
-  <si>
-    <t>高射火炮</t>
-  </si>
-  <si>
-    <t>魔法压制</t>
-  </si>
-  <si>
-    <t>元素压制</t>
-  </si>
-  <si>
-    <t>元素抵抗</t>
-  </si>
-  <si>
-    <t>1020|1021</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1025|1026|1027</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1031|1032|1033</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1029|1030</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1044|1045|1042|1043</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1047|1048|1049</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>基地耐久2</t>
-  </si>
-  <si>
-    <t>敌方减速2</t>
-  </si>
-  <si>
-    <t>矿机升级2</t>
-  </si>
-  <si>
-    <t>天降能量2</t>
-  </si>
-  <si>
-    <t>物理精通</t>
-  </si>
-  <si>
-    <t>魔法升华</t>
-  </si>
-  <si>
-    <t>慧光2</t>
-  </si>
-  <si>
-    <t>慧光3</t>
-  </si>
-  <si>
-    <t>慧光4</t>
-  </si>
-  <si>
-    <t>距离增强2</t>
-  </si>
-  <si>
-    <t>物理斩杀2</t>
-  </si>
-  <si>
-    <t>黯灭2</t>
-  </si>
-  <si>
-    <t>希瓦2</t>
-  </si>
-  <si>
-    <t>高射火炮2</t>
-  </si>
-  <si>
-    <t>魔法压制2</t>
-  </si>
-  <si>
-    <t>物理</t>
-  </si>
-  <si>
-    <t>魔法</t>
-  </si>
-  <si>
-    <t>耐久</t>
-  </si>
-  <si>
-    <t>TalentTree_Name_6</t>
-  </si>
-  <si>
-    <t>光元素增伤</t>
-  </si>
-  <si>
-    <t>攻速增强2</t>
-  </si>
-  <si>
-    <t>iconGray</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>未激活 icon 图标</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1016|1017|1018|1019</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1040|1041|1042</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>耐久恢复2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>光元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>水元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>土元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>暗元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>火元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>木元素增伤2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -897,48 +885,360 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -946,13 +1246,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -962,33 +1504,71 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1238,34 +1818,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="22.375" customWidth="1"/>
     <col min="3" max="3" width="18.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.625" style="1" customWidth="1"/>
     <col min="7" max="8" width="63.375" customWidth="1"/>
-    <col min="10" max="10" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.625" customWidth="1"/>
-    <col min="12" max="12" width="20.5" customWidth="1"/>
-    <col min="13" max="13" width="30" customWidth="1"/>
+    <col min="11" max="11" width="17.625" customWidth="1"/>
+    <col min="12" max="12" width="16.625" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="14" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1291,22 +1871,25 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
       </c>
       <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
       <c r="M1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1334,77 +1917,83 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>108</v>
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" ht="42" customHeight="1" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="42" customHeight="1" spans="1:8">
+      <c r="A4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="5" ht="16.5" spans="1:14">
       <c r="A5" s="1">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1413,36 +2002,39 @@
         <v>1004</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4">
         <v>387109</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
         <v>386997</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>1001</v>
       </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" ht="16.5" spans="1:14">
       <c r="A6" s="1">
         <v>1002</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1451,115 +2043,124 @@
         <v>1004</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
         <v>386998</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>387089</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>1002</v>
       </c>
-      <c r="L6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" ht="16.5" spans="1:14">
       <c r="A7" s="1">
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>182</v>
+      <c r="G7" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
         <v>387015</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>385893</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>1003</v>
       </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" ht="16.5" spans="1:14">
       <c r="A8" s="1">
         <v>1004</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="I8" s="4">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4">
         <v>387108</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>387003</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>1004</v>
       </c>
-      <c r="L8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" ht="16.5" spans="1:14">
       <c r="A9" s="1">
         <v>1005</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1571,36 +2172,39 @@
         <v>1010</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I9" s="4">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4">
         <v>387011</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>387090</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>1005</v>
       </c>
-      <c r="L9" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" ht="16.5" spans="1:14">
       <c r="A10" s="1">
         <v>1006</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>262</v>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1612,36 +2216,39 @@
         <v>1014</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I10" s="4">
+        <v>5</v>
+      </c>
+      <c r="J10" s="4">
         <v>387006</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>387055</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>1006</v>
       </c>
-      <c r="L10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M10" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" ht="16.5" spans="1:14">
       <c r="A11" s="1">
         <v>1007</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>263</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1653,36 +2260,39 @@
         <v>1011</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
         <v>385317</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>385333</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>1007</v>
       </c>
-      <c r="L11" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" spans="1:14">
       <c r="A12" s="1">
         <v>1008</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1694,36 +2304,39 @@
         <v>1012</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I12" s="4">
+        <v>2</v>
+      </c>
+      <c r="J12" s="4">
         <v>385384</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>385288</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>1008</v>
       </c>
-      <c r="L12" t="s">
-        <v>68</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" ht="16.5" spans="1:14">
       <c r="A13" s="1">
         <v>1009</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1735,36 +2348,39 @@
         <v>1013</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I13" s="4">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4">
         <v>385337</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>385284</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>1009</v>
       </c>
-      <c r="L13" t="s">
-        <v>73</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" ht="16.5" spans="1:14">
       <c r="A14" s="1">
         <v>1010</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1776,36 +2392,39 @@
         <v>1014</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I14" s="4">
+        <v>2</v>
+      </c>
+      <c r="J14" s="4">
         <v>387000</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>387058</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>1010</v>
       </c>
-      <c r="L14" t="s">
-        <v>78</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" ht="16.5" spans="1:14">
       <c r="A15" s="1">
         <v>1011</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1817,36 +2436,39 @@
         <v>1015</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I15" s="4">
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
         <v>385331</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <v>385335</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>1011</v>
       </c>
-      <c r="L15" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M15" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" ht="16.5" spans="1:14">
       <c r="A16" s="1">
         <v>1012</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1858,36 +2480,39 @@
         <v>1015</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I16" s="4">
+        <v>2</v>
+      </c>
+      <c r="J16" s="4">
         <v>391472</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>163646</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>1012</v>
       </c>
-      <c r="L16" t="s">
-        <v>88</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M16" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" ht="16.5" spans="1:14">
       <c r="A17" s="1">
         <v>1013</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -1899,118 +2524,127 @@
         <v>1015</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4">
         <v>385338</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>385286</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>1013</v>
       </c>
-      <c r="L17" t="s">
-        <v>93</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" ht="16.5" spans="1:14">
       <c r="A18" s="1">
         <v>1014</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G18" s="1">
         <v>1015</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I18" s="4">
+        <v>3</v>
+      </c>
+      <c r="J18" s="4">
         <v>387013</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>387088</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>1014</v>
       </c>
-      <c r="L18" t="s">
-        <v>99</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M18" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" ht="16.5" spans="1:14">
       <c r="A19" s="1">
         <v>1015</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>267</v>
+        <v>112</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I19" s="4">
+        <v>4</v>
+      </c>
+      <c r="J19" s="4">
         <v>387110</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>387087</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>1015</v>
       </c>
-      <c r="L19" t="s">
-        <v>106</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M19" t="s">
+        <v>115</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" ht="16.5" spans="1:14">
       <c r="A20" s="1">
         <v>1016</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>230</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -2022,36 +2656,39 @@
         <v>1020</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I20" s="4">
+        <v>2</v>
+      </c>
+      <c r="J20" s="4">
         <v>387010</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <v>387086</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>1016</v>
       </c>
-      <c r="L20" t="s">
-        <v>185</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M20" t="s">
+        <v>120</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" ht="16.5" spans="1:14">
       <c r="A21" s="1">
         <v>1017</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -2063,36 +2700,39 @@
         <v>1021</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
         <v>387111</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <v>387005</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>1017</v>
       </c>
-      <c r="L21" t="s">
-        <v>186</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M21" t="s">
+        <v>126</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" ht="16.5" spans="1:14">
       <c r="A22" s="1">
         <v>1018</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>232</v>
+        <v>129</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -2104,36 +2744,39 @@
         <v>1023</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I22" s="4">
+        <v>4</v>
+      </c>
+      <c r="J22" s="4">
         <v>387014</v>
       </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
         <v>387062</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>1018</v>
       </c>
-      <c r="L22" t="s">
-        <v>187</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M22" t="s">
+        <v>131</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" ht="16.5" spans="1:14">
       <c r="A23" s="1">
         <v>1019</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2145,36 +2788,39 @@
         <v>1023</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I23" s="4">
+        <v>4</v>
+      </c>
+      <c r="J23" s="4">
         <v>386996</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>387056</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>1019</v>
       </c>
-      <c r="L23" t="s">
-        <v>188</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M23" t="s">
+        <v>136</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" ht="16.5" spans="1:14">
       <c r="A24" s="1">
         <v>1020</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>234</v>
+        <v>139</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -2186,36 +2832,39 @@
         <v>1022</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I24" s="4">
+        <v>2</v>
+      </c>
+      <c r="J24" s="4">
         <v>387112</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>387084</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>1020</v>
       </c>
-      <c r="L24" t="s">
-        <v>189</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M24" t="s">
+        <v>141</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" ht="16.5" spans="1:14">
       <c r="A25" s="1">
         <v>1021</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>235</v>
+        <v>144</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -2227,159 +2876,171 @@
         <v>1022</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="I25" s="4">
+        <v>1</v>
+      </c>
+      <c r="J25" s="4">
         <v>387107</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>387085</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>1021</v>
       </c>
-      <c r="L25" t="s">
-        <v>190</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M25" t="s">
+        <v>146</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" ht="16.5" spans="1:14">
       <c r="A26" s="1">
         <v>1022</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>236</v>
+        <v>149</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>238</v>
+      <c r="F26" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="G26" s="1">
         <v>1024</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I26" s="4">
+        <v>3</v>
+      </c>
+      <c r="J26" s="4">
         <v>387012</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>387057</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>1022</v>
       </c>
-      <c r="L26" t="s">
-        <v>191</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M26" t="s">
+        <v>152</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" ht="16.5" spans="1:14">
       <c r="A27" s="1">
         <v>1023</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>237</v>
+        <v>155</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G27" s="1">
         <v>1024</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I27" s="4">
+        <v>3</v>
+      </c>
+      <c r="J27" s="4">
         <v>386999</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>387063</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>1023</v>
       </c>
-      <c r="L27" t="s">
-        <v>192</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M27" t="s">
+        <v>158</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" ht="16.5" spans="1:14">
       <c r="A28" s="1">
         <v>1024</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>250</v>
+        <v>160</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>239</v>
+        <v>163</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I28" s="4">
+        <v>4</v>
+      </c>
+      <c r="J28" s="4">
         <v>387110</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>387087</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>1024</v>
       </c>
-      <c r="L28" t="s">
-        <v>193</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M28" t="s">
+        <v>165</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" ht="16.5" spans="1:14">
       <c r="A29" s="1">
         <v>1025</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>248</v>
+        <v>166</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2391,36 +3052,39 @@
         <v>1028</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I29" s="4">
+        <v>3</v>
+      </c>
+      <c r="J29" s="4">
         <v>387109</v>
       </c>
-      <c r="J29" s="4">
+      <c r="K29" s="4">
         <v>386997</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>1025</v>
       </c>
-      <c r="L29" t="s">
-        <v>194</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M29" t="s">
+        <v>169</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" ht="16.5" spans="1:14">
       <c r="A30" s="1">
         <v>1026</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>249</v>
+        <v>170</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2432,36 +3096,39 @@
         <v>1028</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I30" s="4">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4">
         <v>386998</v>
       </c>
-      <c r="J30" s="4">
+      <c r="K30" s="4">
         <v>387089</v>
       </c>
-      <c r="K30" s="1">
+      <c r="L30" s="1">
         <v>1026</v>
       </c>
-      <c r="L30" t="s">
-        <v>195</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M30" t="s">
+        <v>173</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" ht="16.5" spans="1:14">
       <c r="A31" s="1">
         <v>1027</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>244</v>
+        <v>174</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2469,81 +3136,87 @@
       <c r="F31" s="1">
         <v>1024</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>241</v>
+      <c r="G31" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="I31" s="4">
+        <v>3</v>
+      </c>
+      <c r="J31" s="4">
         <v>387015</v>
       </c>
-      <c r="J31" s="4">
+      <c r="K31" s="4">
         <v>385893</v>
       </c>
-      <c r="K31" s="1">
+      <c r="L31" s="1">
         <v>1027</v>
       </c>
-      <c r="L31" t="s">
-        <v>196</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M31" t="s">
+        <v>178</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" ht="16.5" spans="1:14">
       <c r="A32" s="1">
         <v>1028</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>264</v>
+        <v>179</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>240</v>
+        <v>182</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="I32" s="4">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4">
         <v>387108</v>
       </c>
-      <c r="J32" s="4">
+      <c r="K32" s="4">
         <v>387003</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>1028</v>
       </c>
-      <c r="L32" t="s">
-        <v>197</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M32" t="s">
+        <v>184</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" ht="16.5" spans="1:14">
       <c r="A33" s="1">
         <v>1029</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>247</v>
+        <v>185</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -2555,36 +3228,39 @@
         <v>1034</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I33" s="4">
+        <v>2</v>
+      </c>
+      <c r="J33" s="4">
         <v>387011</v>
       </c>
-      <c r="J33" s="4">
+      <c r="K33" s="4">
         <v>387090</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>1029</v>
       </c>
-      <c r="L33" t="s">
-        <v>198</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M33" t="s">
+        <v>188</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" ht="16.5" spans="1:14">
       <c r="A34" s="1">
         <v>1030</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>246</v>
+        <v>189</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2596,36 +3272,39 @@
         <v>1038</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I34" s="4">
+        <v>5</v>
+      </c>
+      <c r="J34" s="4">
         <v>387006</v>
       </c>
-      <c r="J34" s="4">
+      <c r="K34" s="4">
         <v>387055</v>
       </c>
-      <c r="K34" s="1">
+      <c r="L34" s="1">
         <v>1030</v>
       </c>
-      <c r="L34" t="s">
-        <v>199</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M34" t="s">
+        <v>192</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" ht="16.5" spans="1:14">
       <c r="A35" s="1">
         <v>1031</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>270</v>
+        <v>193</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -2637,36 +3316,39 @@
         <v>1035</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I35" s="4">
+        <v>2</v>
+      </c>
+      <c r="J35" s="4">
         <v>385317</v>
       </c>
-      <c r="J35" s="4">
+      <c r="K35" s="4">
         <v>385333</v>
       </c>
-      <c r="K35" s="1">
+      <c r="L35" s="1">
         <v>1031</v>
       </c>
-      <c r="L35" t="s">
-        <v>200</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M35" t="s">
+        <v>196</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" ht="16.5" spans="1:14">
       <c r="A36" s="1">
         <v>1032</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>271</v>
+        <v>197</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -2678,36 +3360,39 @@
         <v>1036</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I36" s="4">
+        <v>2</v>
+      </c>
+      <c r="J36" s="4">
         <v>385384</v>
       </c>
-      <c r="J36" s="4">
+      <c r="K36" s="4">
         <v>385288</v>
       </c>
-      <c r="K36" s="1">
+      <c r="L36" s="1">
         <v>1032</v>
       </c>
-      <c r="L36" t="s">
-        <v>201</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M36" t="s">
+        <v>200</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" ht="16.5" spans="1:14">
       <c r="A37" s="1">
         <v>1033</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>272</v>
+        <v>201</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -2719,36 +3404,39 @@
         <v>1037</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I37" s="4">
+        <v>2</v>
+      </c>
+      <c r="J37" s="4">
         <v>385337</v>
       </c>
-      <c r="J37" s="4">
+      <c r="K37" s="4">
         <v>385284</v>
       </c>
-      <c r="K37" s="1">
+      <c r="L37" s="1">
         <v>1033</v>
       </c>
-      <c r="L37" t="s">
-        <v>202</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M37" t="s">
+        <v>204</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" ht="16.5" spans="1:14">
       <c r="A38" s="1">
         <v>1034</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>269</v>
+        <v>205</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -2760,36 +3448,39 @@
         <v>1038</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I38" s="4">
+        <v>2</v>
+      </c>
+      <c r="J38" s="4">
         <v>387000</v>
       </c>
-      <c r="J38" s="4">
+      <c r="K38" s="4">
         <v>387058</v>
       </c>
-      <c r="K38" s="1">
+      <c r="L38" s="1">
         <v>1034</v>
       </c>
-      <c r="L38" t="s">
-        <v>203</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M38" t="s">
+        <v>208</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" ht="16.5" spans="1:14">
       <c r="A39" s="1">
         <v>1035</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>273</v>
+        <v>209</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -2801,36 +3492,39 @@
         <v>1039</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I39" s="4">
+        <v>2</v>
+      </c>
+      <c r="J39" s="4">
         <v>385331</v>
       </c>
-      <c r="J39" s="4">
+      <c r="K39" s="4">
         <v>385335</v>
       </c>
-      <c r="K39" s="1">
+      <c r="L39" s="1">
         <v>1035</v>
       </c>
-      <c r="L39" t="s">
-        <v>204</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M39" t="s">
+        <v>212</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" ht="16.5" spans="1:14">
       <c r="A40" s="1">
         <v>1036</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>274</v>
+        <v>213</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -2842,36 +3536,39 @@
         <v>1039</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I40" s="4">
+        <v>2</v>
+      </c>
+      <c r="J40" s="4">
         <v>391472</v>
       </c>
-      <c r="J40" s="4">
+      <c r="K40" s="4">
         <v>163646</v>
       </c>
-      <c r="K40" s="1">
+      <c r="L40" s="1">
         <v>1036</v>
       </c>
-      <c r="L40" t="s">
-        <v>205</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M40" t="s">
+        <v>216</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" ht="16.5" spans="1:14">
       <c r="A41" s="1">
         <v>1037</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>275</v>
+        <v>217</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -2883,118 +3580,127 @@
         <v>1039</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I41" s="4">
+        <v>2</v>
+      </c>
+      <c r="J41" s="4">
         <v>385338</v>
       </c>
-      <c r="J41" s="4">
+      <c r="K41" s="4">
         <v>385286</v>
       </c>
-      <c r="K41" s="1">
+      <c r="L41" s="1">
         <v>1037</v>
       </c>
-      <c r="L41" t="s">
-        <v>206</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M41" t="s">
+        <v>220</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" ht="16.5" spans="1:14">
       <c r="A42" s="1">
         <v>1038</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>245</v>
+        <v>221</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>165</v>
+        <v>223</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="G42" s="1">
         <v>1039</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I42" s="4">
+        <v>3</v>
+      </c>
+      <c r="J42" s="4">
         <v>387013</v>
       </c>
-      <c r="J42" s="4">
+      <c r="K42" s="4">
         <v>387088</v>
       </c>
-      <c r="K42" s="1">
+      <c r="L42" s="1">
         <v>1038</v>
       </c>
-      <c r="L42" t="s">
-        <v>207</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M42" t="s">
+        <v>225</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" ht="16.5" spans="1:14">
       <c r="A43" s="1">
         <v>1039</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>251</v>
+        <v>226</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>166</v>
+        <v>228</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>268</v>
+        <v>229</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I43" s="4">
+        <v>4</v>
+      </c>
+      <c r="J43" s="4">
         <v>387110</v>
       </c>
-      <c r="J43" s="4">
+      <c r="K43" s="4">
         <v>387087</v>
       </c>
-      <c r="K43" s="1">
+      <c r="L43" s="1">
         <v>1039</v>
       </c>
-      <c r="L43" t="s">
-        <v>208</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M43" t="s">
+        <v>231</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" ht="16.5" spans="1:14">
       <c r="A44" s="1">
         <v>1040</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>253</v>
+        <v>232</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>167</v>
+        <v>234</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -3006,36 +3712,39 @@
         <v>1044</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I44" s="4">
+        <v>2</v>
+      </c>
+      <c r="J44" s="4">
         <v>387010</v>
       </c>
-      <c r="J44" s="4">
+      <c r="K44" s="4">
         <v>387086</v>
       </c>
-      <c r="K44" s="1">
+      <c r="L44" s="1">
         <v>1040</v>
       </c>
-      <c r="L44" t="s">
-        <v>209</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M44" t="s">
+        <v>235</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" ht="16.5" spans="1:14">
       <c r="A45" s="1">
         <v>1041</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>254</v>
+        <v>236</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>168</v>
+        <v>238</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -3047,36 +3756,39 @@
         <v>1045</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="I45" s="4">
+        <v>1</v>
+      </c>
+      <c r="J45" s="4">
         <v>387111</v>
       </c>
-      <c r="J45" s="4">
+      <c r="K45" s="4">
         <v>387005</v>
       </c>
-      <c r="K45" s="1">
+      <c r="L45" s="1">
         <v>1041</v>
       </c>
-      <c r="L45" t="s">
-        <v>210</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M45" t="s">
+        <v>239</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" ht="16.5" spans="1:14">
       <c r="A46" s="1">
         <v>1042</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>255</v>
+        <v>240</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>169</v>
+        <v>242</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -3088,36 +3800,39 @@
         <v>1046</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I46" s="4">
+        <v>4</v>
+      </c>
+      <c r="J46" s="4">
         <v>387014</v>
       </c>
-      <c r="J46" s="4">
+      <c r="K46" s="4">
         <v>387062</v>
       </c>
-      <c r="K46" s="1">
+      <c r="L46" s="1">
         <v>1042</v>
       </c>
-      <c r="L46" t="s">
-        <v>211</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M46" t="s">
+        <v>243</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" ht="16.5" spans="1:14">
       <c r="A47" s="1">
         <v>1043</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>256</v>
+        <v>244</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -3129,36 +3844,39 @@
         <v>1046</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I47" s="4">
+        <v>4</v>
+      </c>
+      <c r="J47" s="4">
         <v>386996</v>
       </c>
-      <c r="J47" s="4">
+      <c r="K47" s="4">
         <v>387056</v>
       </c>
-      <c r="K47" s="1">
+      <c r="L47" s="1">
         <v>1043</v>
       </c>
-      <c r="L47" t="s">
-        <v>212</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M47" t="s">
+        <v>247</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" ht="16.5" spans="1:14">
       <c r="A48" s="1">
         <v>1044</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>257</v>
+        <v>248</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>171</v>
+        <v>250</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -3170,36 +3888,39 @@
         <v>1046</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I48" s="4">
+        <v>2</v>
+      </c>
+      <c r="J48" s="4">
         <v>387112</v>
       </c>
-      <c r="J48" s="4">
+      <c r="K48" s="4">
         <v>387084</v>
       </c>
-      <c r="K48" s="1">
+      <c r="L48" s="1">
         <v>1044</v>
       </c>
-      <c r="L48" t="s">
-        <v>213</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M48" t="s">
+        <v>251</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" ht="16.5" spans="1:14">
       <c r="A49" s="1">
         <v>1045</v>
       </c>
       <c r="B49" t="s">
-        <v>138</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -3211,77 +3932,83 @@
         <v>1046</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="I49" s="4">
+        <v>1</v>
+      </c>
+      <c r="J49" s="4">
         <v>387107</v>
       </c>
-      <c r="J49" s="4">
+      <c r="K49" s="4">
         <v>387085</v>
       </c>
-      <c r="K49" s="1">
+      <c r="L49" s="1">
         <v>1045</v>
       </c>
-      <c r="L49" t="s">
-        <v>214</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M49" t="s">
+        <v>255</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" ht="16.5" spans="1:14">
       <c r="A50" s="1">
         <v>1046</v>
       </c>
       <c r="B50" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>252</v>
+        <v>256</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>173</v>
+        <v>258</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>243</v>
+      <c r="F50" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I50" s="4">
+        <v>4</v>
+      </c>
+      <c r="J50" s="4">
         <v>387012</v>
       </c>
-      <c r="J50" s="4">
+      <c r="K50" s="4">
         <v>387057</v>
       </c>
-      <c r="K50" s="1">
+      <c r="L50" s="1">
         <v>1046</v>
       </c>
-      <c r="L50" t="s">
-        <v>215</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M50" t="s">
+        <v>261</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" ht="16.5" spans="1:14">
       <c r="A51" s="1">
         <v>1047</v>
       </c>
       <c r="B51" t="s">
-        <v>140</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -3289,37 +4016,40 @@
       <c r="F51" s="1">
         <v>1046</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>184</v>
+      <c r="H51" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="I51" s="4">
+        <v>10</v>
+      </c>
+      <c r="J51" s="4">
         <v>387007</v>
       </c>
-      <c r="J51" s="4">
+      <c r="K51" s="4">
         <v>387060</v>
       </c>
-      <c r="K51" s="1">
+      <c r="L51" s="1">
         <v>1047</v>
       </c>
-      <c r="L51" t="s">
-        <v>216</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M51" t="s">
+        <v>266</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" ht="16.5" spans="1:14">
       <c r="A52" s="1">
         <v>1048</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>260</v>
+        <v>268</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>175</v>
+        <v>270</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -3327,37 +4057,40 @@
       <c r="F52" s="1">
         <v>1046</v>
       </c>
-      <c r="H52" s="6" t="s">
-        <v>184</v>
+      <c r="H52" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="I52" s="4">
+        <v>10</v>
+      </c>
+      <c r="J52" s="4">
         <v>387002</v>
       </c>
-      <c r="J52" s="4">
+      <c r="K52" s="4">
         <v>387059</v>
       </c>
-      <c r="K52" s="1">
+      <c r="L52" s="1">
         <v>1048</v>
       </c>
-      <c r="L52" t="s">
-        <v>217</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="M52" t="s">
+        <v>271</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" ht="16.5" spans="1:14">
       <c r="A53" s="1">
         <v>1049</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>261</v>
+        <v>273</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>176</v>
+        <v>275</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -3365,28 +4098,31 @@
       <c r="F53" s="1">
         <v>1046</v>
       </c>
-      <c r="H53" s="6" t="s">
-        <v>184</v>
+      <c r="H53" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="I53" s="4">
+        <v>10</v>
+      </c>
+      <c r="J53" s="4">
         <v>387004</v>
       </c>
-      <c r="J53" s="4">
+      <c r="K53" s="4">
         <v>387061</v>
       </c>
-      <c r="K53" s="1">
+      <c r="L53" s="1">
         <v>1049</v>
       </c>
-      <c r="L53" t="s">
-        <v>218</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>229</v>
+      <c r="M53" t="s">
+        <v>276</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add maxlevel ui
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -719,7 +719,7 @@
     <t>1035|1036|1037|1038</t>
   </si>
   <si>
-    <t>1040|1041|1042</t>
+    <t>1040|1041|1042|1043</t>
   </si>
   <si>
     <t>TalentTree_Desc_39</t>
@@ -873,14 +873,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1364,133 +1357,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1501,16 +1494,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1826,8 +1819,8 @@
   <sheetPr/>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
feat: add talent config
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="288">
   <si>
     <t>int</t>
   </si>
@@ -41,6 +41,12 @@
     <t>int[][]</t>
   </si>
   <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>float[]</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -74,6 +80,15 @@
     <t>iconGray</t>
   </si>
   <si>
+    <t>iconSize</t>
+  </si>
+  <si>
+    <t>iconPos</t>
+  </si>
+  <si>
+    <t>outlineColor</t>
+  </si>
+  <si>
     <t>buffId</t>
   </si>
   <si>
@@ -116,6 +131,15 @@
     <t>未激活 icon 图标</t>
   </si>
   <si>
+    <t>icon大小</t>
+  </si>
+  <si>
+    <t>icon位置</t>
+  </si>
+  <si>
+    <t>字体描边颜色</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 天赋buff表的id</t>
   </si>
   <si>
@@ -135,6 +159,12 @@
   </si>
   <si>
     <t>1|10|20||2|10|20</t>
+  </si>
+  <si>
+    <t>12.5|-2</t>
+  </si>
+  <si>
+    <t>#63220F</t>
   </si>
   <si>
     <t>TalentTree_Desc_1</t>
@@ -1817,10 +1847,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1833,12 +1863,12 @@
     <col min="6" max="6" width="21.625" style="1" customWidth="1"/>
     <col min="7" max="8" width="63.375" customWidth="1"/>
     <col min="11" max="11" width="17.625" customWidth="1"/>
-    <col min="12" max="12" width="16.625" customWidth="1"/>
-    <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
+    <col min="12" max="15" width="16.625" customWidth="1"/>
+    <col min="16" max="16" width="20.5" customWidth="1"/>
+    <col min="17" max="17" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1873,101 +1903,128 @@
         <v>1</v>
       </c>
       <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" ht="42" customHeight="1" spans="1:14">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" ht="42" customHeight="1" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="42" customHeight="1" spans="1:8">
@@ -1975,18 +2032,18 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" ht="16.5" spans="1:14">
+    <row r="5" ht="16.5" spans="1:17">
       <c r="A5" s="1">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1995,7 +2052,7 @@
         <v>1004</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I5" s="4">
         <v>2</v>
@@ -2007,27 +2064,36 @@
         <v>386997</v>
       </c>
       <c r="L5" s="1">
+        <v>48</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="1">
         <v>1001</v>
       </c>
-      <c r="M5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" ht="16.5" spans="1:14">
+      <c r="P5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" ht="16.5" spans="1:17">
       <c r="A6" s="1">
         <v>1002</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -2036,7 +2102,7 @@
         <v>1004</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I6" s="4">
         <v>2</v>
@@ -2048,36 +2114,45 @@
         <v>387089</v>
       </c>
       <c r="L6" s="1">
+        <v>48</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="1">
         <v>1002</v>
       </c>
-      <c r="M6" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" ht="16.5" spans="1:14">
+      <c r="P6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" ht="16.5" spans="1:17">
       <c r="A7" s="1">
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I7" s="4">
         <v>3</v>
@@ -2089,39 +2164,48 @@
         <v>385893</v>
       </c>
       <c r="L7" s="1">
+        <v>48</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="1">
         <v>1003</v>
       </c>
-      <c r="M7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" ht="16.5" spans="1:14">
+      <c r="P7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" ht="16.5" spans="1:17">
       <c r="A8" s="1">
         <v>1004</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4">
         <v>3</v>
@@ -2133,27 +2217,36 @@
         <v>387003</v>
       </c>
       <c r="L8" s="1">
+        <v>48</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="1">
         <v>1004</v>
       </c>
-      <c r="M8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" ht="16.5" spans="1:14">
+      <c r="P8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" ht="16.5" spans="1:17">
       <c r="A9" s="1">
         <v>1005</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -2165,7 +2258,7 @@
         <v>1010</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -2177,27 +2270,36 @@
         <v>387090</v>
       </c>
       <c r="L9" s="1">
+        <v>48</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="1">
         <v>1005</v>
       </c>
-      <c r="M9" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" spans="1:14">
+      <c r="P9" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" ht="16.5" spans="1:17">
       <c r="A10" s="1">
         <v>1006</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -2209,7 +2311,7 @@
         <v>1014</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="I10" s="4">
         <v>5</v>
@@ -2221,27 +2323,36 @@
         <v>387055</v>
       </c>
       <c r="L10" s="1">
+        <v>48</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="1">
         <v>1006</v>
       </c>
-      <c r="M10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" ht="16.5" spans="1:14">
+      <c r="P10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" ht="16.5" spans="1:17">
       <c r="A11" s="1">
         <v>1007</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2253,7 +2364,7 @@
         <v>1011</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I11" s="4">
         <v>2</v>
@@ -2265,27 +2376,36 @@
         <v>385333</v>
       </c>
       <c r="L11" s="1">
+        <v>48</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="1">
         <v>1007</v>
       </c>
-      <c r="M11" t="s">
-        <v>71</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" ht="16.5" spans="1:14">
+      <c r="P11" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" spans="1:17">
       <c r="A12" s="1">
         <v>1008</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -2297,7 +2417,7 @@
         <v>1012</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I12" s="4">
         <v>2</v>
@@ -2309,27 +2429,36 @@
         <v>385288</v>
       </c>
       <c r="L12" s="1">
+        <v>48</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="1">
         <v>1008</v>
       </c>
-      <c r="M12" t="s">
-        <v>76</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" ht="16.5" spans="1:14">
+      <c r="P12" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" ht="16.5" spans="1:17">
       <c r="A13" s="1">
         <v>1009</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -2341,7 +2470,7 @@
         <v>1013</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I13" s="4">
         <v>2</v>
@@ -2353,27 +2482,36 @@
         <v>385284</v>
       </c>
       <c r="L13" s="1">
+        <v>48</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13" s="1">
         <v>1009</v>
       </c>
-      <c r="M13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" ht="16.5" spans="1:14">
+      <c r="P13" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" ht="16.5" spans="1:17">
       <c r="A14" s="1">
         <v>1010</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -2385,7 +2523,7 @@
         <v>1014</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
@@ -2397,27 +2535,36 @@
         <v>387058</v>
       </c>
       <c r="L14" s="1">
+        <v>48</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14" s="1">
         <v>1010</v>
       </c>
-      <c r="M14" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" ht="16.5" spans="1:14">
+      <c r="P14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" ht="16.5" spans="1:17">
       <c r="A15" s="1">
         <v>1011</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -2429,7 +2576,7 @@
         <v>1015</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I15" s="4">
         <v>2</v>
@@ -2441,27 +2588,36 @@
         <v>385335</v>
       </c>
       <c r="L15" s="1">
+        <v>48</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" s="1">
         <v>1011</v>
       </c>
-      <c r="M15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" ht="16.5" spans="1:14">
+      <c r="P15" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" ht="16.5" spans="1:17">
       <c r="A16" s="1">
         <v>1012</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2473,7 +2629,7 @@
         <v>1015</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I16" s="4">
         <v>2</v>
@@ -2485,27 +2641,36 @@
         <v>163646</v>
       </c>
       <c r="L16" s="1">
+        <v>48</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" s="1">
         <v>1012</v>
       </c>
-      <c r="M16" t="s">
-        <v>96</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" ht="16.5" spans="1:14">
+      <c r="P16" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" ht="16.5" spans="1:17">
       <c r="A17" s="1">
         <v>1013</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2517,7 +2682,7 @@
         <v>1015</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I17" s="4">
         <v>2</v>
@@ -2529,39 +2694,48 @@
         <v>385286</v>
       </c>
       <c r="L17" s="1">
+        <v>48</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="1">
         <v>1013</v>
       </c>
-      <c r="M17" t="s">
-        <v>101</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" ht="16.5" spans="1:14">
+      <c r="P17" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" ht="16.5" spans="1:17">
       <c r="A18" s="1">
         <v>1014</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="G18" s="1">
         <v>1015</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I18" s="4">
         <v>3</v>
@@ -2573,39 +2747,48 @@
         <v>387088</v>
       </c>
       <c r="L18" s="1">
+        <v>48</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18" s="1">
         <v>1014</v>
       </c>
-      <c r="M18" t="s">
-        <v>107</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" ht="16.5" spans="1:14">
+      <c r="P18" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" ht="16.5" spans="1:17">
       <c r="A19" s="1">
         <v>1015</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I19" s="4">
         <v>4</v>
@@ -2617,27 +2800,36 @@
         <v>387087</v>
       </c>
       <c r="L19" s="1">
+        <v>48</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="1">
         <v>1015</v>
       </c>
-      <c r="M19" t="s">
-        <v>115</v>
-      </c>
-      <c r="N19" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" ht="16.5" spans="1:14">
+      <c r="P19" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" ht="16.5" spans="1:17">
       <c r="A20" s="1">
         <v>1016</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -2649,7 +2841,7 @@
         <v>1020</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I20" s="4">
         <v>2</v>
@@ -2661,27 +2853,36 @@
         <v>387086</v>
       </c>
       <c r="L20" s="1">
+        <v>48</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="1">
         <v>1016</v>
       </c>
-      <c r="M20" t="s">
-        <v>120</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" ht="16.5" spans="1:14">
+      <c r="P20" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" ht="16.5" spans="1:17">
       <c r="A21" s="1">
         <v>1017</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -2693,7 +2894,7 @@
         <v>1021</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I21" s="4">
         <v>1</v>
@@ -2705,27 +2906,36 @@
         <v>387005</v>
       </c>
       <c r="L21" s="1">
+        <v>48</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="1">
         <v>1017</v>
       </c>
-      <c r="M21" t="s">
-        <v>126</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" ht="16.5" spans="1:14">
+      <c r="P21" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" ht="16.5" spans="1:17">
       <c r="A22" s="1">
         <v>1018</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -2737,7 +2947,7 @@
         <v>1023</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I22" s="4">
         <v>4</v>
@@ -2749,27 +2959,36 @@
         <v>387062</v>
       </c>
       <c r="L22" s="1">
+        <v>48</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" s="1">
         <v>1018</v>
       </c>
-      <c r="M22" t="s">
-        <v>131</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" ht="16.5" spans="1:14">
+      <c r="P22" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" ht="16.5" spans="1:17">
       <c r="A23" s="1">
         <v>1019</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2781,7 +3000,7 @@
         <v>1023</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I23" s="4">
         <v>4</v>
@@ -2793,27 +3012,36 @@
         <v>387056</v>
       </c>
       <c r="L23" s="1">
+        <v>48</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" s="1">
         <v>1019</v>
       </c>
-      <c r="M23" t="s">
-        <v>136</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" ht="16.5" spans="1:14">
+      <c r="P23" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" ht="16.5" spans="1:17">
       <c r="A24" s="1">
         <v>1020</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -2825,7 +3053,7 @@
         <v>1022</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I24" s="4">
         <v>2</v>
@@ -2837,27 +3065,36 @@
         <v>387084</v>
       </c>
       <c r="L24" s="1">
+        <v>48</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" s="1">
         <v>1020</v>
       </c>
-      <c r="M24" t="s">
-        <v>141</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" ht="16.5" spans="1:14">
+      <c r="P24" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" ht="16.5" spans="1:17">
       <c r="A25" s="1">
         <v>1021</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -2869,7 +3106,7 @@
         <v>1022</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I25" s="4">
         <v>1</v>
@@ -2881,39 +3118,48 @@
         <v>387085</v>
       </c>
       <c r="L25" s="1">
+        <v>48</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O25" s="1">
         <v>1021</v>
       </c>
-      <c r="M25" t="s">
-        <v>146</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" ht="16.5" spans="1:14">
+      <c r="P25" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" ht="16.5" spans="1:17">
       <c r="A26" s="1">
         <v>1022</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G26" s="1">
         <v>1024</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I26" s="4">
         <v>3</v>
@@ -2925,39 +3171,48 @@
         <v>387057</v>
       </c>
       <c r="L26" s="1">
+        <v>48</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O26" s="1">
         <v>1022</v>
       </c>
-      <c r="M26" t="s">
-        <v>152</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" ht="16.5" spans="1:14">
+      <c r="P26" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" ht="16.5" spans="1:17">
       <c r="A27" s="1">
         <v>1023</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G27" s="1">
         <v>1024</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I27" s="4">
         <v>3</v>
@@ -2969,39 +3224,48 @@
         <v>387063</v>
       </c>
       <c r="L27" s="1">
+        <v>48</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O27" s="1">
         <v>1023</v>
       </c>
-      <c r="M27" t="s">
-        <v>158</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" ht="16.5" spans="1:14">
+      <c r="P27" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" ht="16.5" spans="1:17">
       <c r="A28" s="1">
         <v>1024</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I28" s="4">
         <v>4</v>
@@ -3013,27 +3277,36 @@
         <v>387087</v>
       </c>
       <c r="L28" s="1">
+        <v>48</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28" s="1">
         <v>1024</v>
       </c>
-      <c r="M28" t="s">
-        <v>165</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" ht="16.5" spans="1:14">
+      <c r="P28" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" ht="16.5" spans="1:17">
       <c r="A29" s="1">
         <v>1025</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -3045,7 +3318,7 @@
         <v>1028</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I29" s="4">
         <v>3</v>
@@ -3057,27 +3330,36 @@
         <v>386997</v>
       </c>
       <c r="L29" s="1">
+        <v>48</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29" s="1">
         <v>1025</v>
       </c>
-      <c r="M29" t="s">
-        <v>169</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" ht="16.5" spans="1:14">
+      <c r="P29" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" ht="16.5" spans="1:17">
       <c r="A30" s="1">
         <v>1026</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -3089,7 +3371,7 @@
         <v>1028</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I30" s="4">
         <v>3</v>
@@ -3101,27 +3383,36 @@
         <v>387089</v>
       </c>
       <c r="L30" s="1">
+        <v>48</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O30" s="1">
         <v>1026</v>
       </c>
-      <c r="M30" t="s">
-        <v>173</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" ht="16.5" spans="1:14">
+      <c r="P30" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" ht="16.5" spans="1:17">
       <c r="A31" s="1">
         <v>1027</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -3130,10 +3421,10 @@
         <v>1024</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I31" s="4">
         <v>3</v>
@@ -3145,39 +3436,48 @@
         <v>385893</v>
       </c>
       <c r="L31" s="1">
+        <v>48</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O31" s="1">
         <v>1027</v>
       </c>
-      <c r="M31" t="s">
-        <v>178</v>
-      </c>
-      <c r="N31" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" ht="16.5" spans="1:14">
+      <c r="P31" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q31" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" ht="16.5" spans="1:17">
       <c r="A32" s="1">
         <v>1028</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I32" s="4">
         <v>3</v>
@@ -3189,27 +3489,36 @@
         <v>387003</v>
       </c>
       <c r="L32" s="1">
+        <v>48</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32" s="1">
         <v>1028</v>
       </c>
-      <c r="M32" t="s">
-        <v>184</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" ht="16.5" spans="1:14">
+      <c r="P32" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" ht="16.5" spans="1:17">
       <c r="A33" s="1">
         <v>1029</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -3221,7 +3530,7 @@
         <v>1034</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I33" s="4">
         <v>2</v>
@@ -3233,27 +3542,36 @@
         <v>387090</v>
       </c>
       <c r="L33" s="1">
+        <v>48</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O33" s="1">
         <v>1029</v>
       </c>
-      <c r="M33" t="s">
-        <v>188</v>
-      </c>
-      <c r="N33" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" ht="16.5" spans="1:14">
+      <c r="P33" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" ht="16.5" spans="1:17">
       <c r="A34" s="1">
         <v>1030</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -3265,7 +3583,7 @@
         <v>1038</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="I34" s="4">
         <v>5</v>
@@ -3277,27 +3595,36 @@
         <v>387055</v>
       </c>
       <c r="L34" s="1">
+        <v>48</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O34" s="1">
         <v>1030</v>
       </c>
-      <c r="M34" t="s">
-        <v>192</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" ht="16.5" spans="1:14">
+      <c r="P34" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" ht="16.5" spans="1:17">
       <c r="A35" s="1">
         <v>1031</v>
       </c>
       <c r="B35" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -3309,7 +3636,7 @@
         <v>1035</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I35" s="4">
         <v>2</v>
@@ -3321,27 +3648,36 @@
         <v>385333</v>
       </c>
       <c r="L35" s="1">
+        <v>48</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O35" s="1">
         <v>1031</v>
       </c>
-      <c r="M35" t="s">
-        <v>196</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" ht="16.5" spans="1:14">
+      <c r="P35" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" ht="16.5" spans="1:17">
       <c r="A36" s="1">
         <v>1032</v>
       </c>
       <c r="B36" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -3353,7 +3689,7 @@
         <v>1036</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I36" s="4">
         <v>2</v>
@@ -3365,27 +3701,36 @@
         <v>385288</v>
       </c>
       <c r="L36" s="1">
+        <v>48</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36" s="1">
         <v>1032</v>
       </c>
-      <c r="M36" t="s">
-        <v>200</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" ht="16.5" spans="1:14">
+      <c r="P36" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" ht="16.5" spans="1:17">
       <c r="A37" s="1">
         <v>1033</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -3397,7 +3742,7 @@
         <v>1037</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I37" s="4">
         <v>2</v>
@@ -3409,27 +3754,36 @@
         <v>385284</v>
       </c>
       <c r="L37" s="1">
+        <v>48</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37" s="1">
         <v>1033</v>
       </c>
-      <c r="M37" t="s">
-        <v>204</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" ht="16.5" spans="1:14">
+      <c r="P37" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" ht="16.5" spans="1:17">
       <c r="A38" s="1">
         <v>1034</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -3441,7 +3795,7 @@
         <v>1038</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I38" s="4">
         <v>2</v>
@@ -3453,27 +3807,36 @@
         <v>387058</v>
       </c>
       <c r="L38" s="1">
+        <v>48</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O38" s="1">
         <v>1034</v>
       </c>
-      <c r="M38" t="s">
-        <v>208</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" ht="16.5" spans="1:14">
+      <c r="P38" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" ht="16.5" spans="1:17">
       <c r="A39" s="1">
         <v>1035</v>
       </c>
       <c r="B39" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -3485,7 +3848,7 @@
         <v>1039</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I39" s="4">
         <v>2</v>
@@ -3497,27 +3860,36 @@
         <v>385335</v>
       </c>
       <c r="L39" s="1">
+        <v>48</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O39" s="1">
         <v>1035</v>
       </c>
-      <c r="M39" t="s">
-        <v>212</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" ht="16.5" spans="1:14">
+      <c r="P39" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" ht="16.5" spans="1:17">
       <c r="A40" s="1">
         <v>1036</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -3529,7 +3901,7 @@
         <v>1039</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I40" s="4">
         <v>2</v>
@@ -3541,27 +3913,36 @@
         <v>163646</v>
       </c>
       <c r="L40" s="1">
+        <v>48</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O40" s="1">
         <v>1036</v>
       </c>
-      <c r="M40" t="s">
-        <v>216</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" ht="16.5" spans="1:14">
+      <c r="P40" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" ht="16.5" spans="1:17">
       <c r="A41" s="1">
         <v>1037</v>
       </c>
       <c r="B41" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -3573,7 +3954,7 @@
         <v>1039</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I41" s="4">
         <v>2</v>
@@ -3585,39 +3966,48 @@
         <v>385286</v>
       </c>
       <c r="L41" s="1">
+        <v>48</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O41" s="1">
         <v>1037</v>
       </c>
-      <c r="M41" t="s">
-        <v>220</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" ht="16.5" spans="1:14">
+      <c r="P41" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" ht="16.5" spans="1:17">
       <c r="A42" s="1">
         <v>1038</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="G42" s="1">
         <v>1039</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I42" s="4">
         <v>3</v>
@@ -3629,39 +4019,48 @@
         <v>387088</v>
       </c>
       <c r="L42" s="1">
+        <v>48</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O42" s="1">
         <v>1038</v>
       </c>
-      <c r="M42" t="s">
-        <v>225</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" ht="16.5" spans="1:14">
+      <c r="P42" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" ht="16.5" spans="1:17">
       <c r="A43" s="1">
         <v>1039</v>
       </c>
       <c r="B43" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I43" s="4">
         <v>4</v>
@@ -3673,27 +4072,36 @@
         <v>387087</v>
       </c>
       <c r="L43" s="1">
+        <v>48</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O43" s="1">
         <v>1039</v>
       </c>
-      <c r="M43" t="s">
-        <v>231</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" ht="16.5" spans="1:14">
+      <c r="P43" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" ht="16.5" spans="1:17">
       <c r="A44" s="1">
         <v>1040</v>
       </c>
       <c r="B44" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -3705,7 +4113,7 @@
         <v>1044</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I44" s="4">
         <v>2</v>
@@ -3717,27 +4125,36 @@
         <v>387086</v>
       </c>
       <c r="L44" s="1">
+        <v>48</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O44" s="1">
         <v>1040</v>
       </c>
-      <c r="M44" t="s">
-        <v>235</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" ht="16.5" spans="1:14">
+      <c r="P44" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" ht="16.5" spans="1:17">
       <c r="A45" s="1">
         <v>1041</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -3749,7 +4166,7 @@
         <v>1045</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I45" s="4">
         <v>1</v>
@@ -3761,27 +4178,36 @@
         <v>387005</v>
       </c>
       <c r="L45" s="1">
+        <v>48</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O45" s="1">
         <v>1041</v>
       </c>
-      <c r="M45" t="s">
-        <v>239</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" ht="16.5" spans="1:14">
+      <c r="P45" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" ht="16.5" spans="1:17">
       <c r="A46" s="1">
         <v>1042</v>
       </c>
       <c r="B46" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -3793,7 +4219,7 @@
         <v>1046</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I46" s="4">
         <v>4</v>
@@ -3805,27 +4231,36 @@
         <v>387062</v>
       </c>
       <c r="L46" s="1">
+        <v>48</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O46" s="1">
         <v>1042</v>
       </c>
-      <c r="M46" t="s">
-        <v>243</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" ht="16.5" spans="1:14">
+      <c r="P46" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" ht="16.5" spans="1:17">
       <c r="A47" s="1">
         <v>1043</v>
       </c>
       <c r="B47" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -3837,7 +4272,7 @@
         <v>1046</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I47" s="4">
         <v>4</v>
@@ -3849,27 +4284,36 @@
         <v>387056</v>
       </c>
       <c r="L47" s="1">
+        <v>48</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O47" s="1">
         <v>1043</v>
       </c>
-      <c r="M47" t="s">
-        <v>247</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" ht="16.5" spans="1:14">
+      <c r="P47" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" ht="16.5" spans="1:17">
       <c r="A48" s="1">
         <v>1044</v>
       </c>
       <c r="B48" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -3881,7 +4325,7 @@
         <v>1046</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="I48" s="4">
         <v>2</v>
@@ -3893,27 +4337,36 @@
         <v>387084</v>
       </c>
       <c r="L48" s="1">
+        <v>48</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O48" s="1">
         <v>1044</v>
       </c>
-      <c r="M48" t="s">
-        <v>251</v>
-      </c>
-      <c r="N48" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" ht="16.5" spans="1:14">
+      <c r="P48" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" ht="16.5" spans="1:17">
       <c r="A49" s="1">
         <v>1045</v>
       </c>
       <c r="B49" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -3925,7 +4378,7 @@
         <v>1046</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="I49" s="4">
         <v>1</v>
@@ -3937,39 +4390,48 @@
         <v>387085</v>
       </c>
       <c r="L49" s="1">
+        <v>48</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O49" s="1">
         <v>1045</v>
       </c>
-      <c r="M49" t="s">
-        <v>255</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" ht="16.5" spans="1:14">
+      <c r="P49" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" ht="16.5" spans="1:17">
       <c r="A50" s="1">
         <v>1046</v>
       </c>
       <c r="B50" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I50" s="4">
         <v>4</v>
@@ -3981,27 +4443,36 @@
         <v>387057</v>
       </c>
       <c r="L50" s="1">
+        <v>48</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O50" s="1">
         <v>1046</v>
       </c>
-      <c r="M50" t="s">
-        <v>261</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="51" ht="16.5" spans="1:14">
+      <c r="P50" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" ht="16.5" spans="1:17">
       <c r="A51" s="1">
         <v>1047</v>
       </c>
       <c r="B51" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -4010,7 +4481,7 @@
         <v>1046</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="I51" s="4">
         <v>10</v>
@@ -4022,27 +4493,36 @@
         <v>387060</v>
       </c>
       <c r="L51" s="1">
+        <v>48</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O51" s="1">
         <v>1047</v>
       </c>
-      <c r="M51" t="s">
-        <v>266</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="52" ht="16.5" spans="1:14">
+      <c r="P51" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" ht="16.5" spans="1:17">
       <c r="A52" s="1">
         <v>1048</v>
       </c>
       <c r="B52" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -4051,7 +4531,7 @@
         <v>1046</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="I52" s="4">
         <v>10</v>
@@ -4063,27 +4543,36 @@
         <v>387059</v>
       </c>
       <c r="L52" s="1">
+        <v>48</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O52" s="1">
         <v>1048</v>
       </c>
-      <c r="M52" t="s">
-        <v>271</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="53" ht="16.5" spans="1:14">
+      <c r="P52" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" ht="16.5" spans="1:17">
       <c r="A53" s="1">
         <v>1049</v>
       </c>
       <c r="B53" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -4092,7 +4581,7 @@
         <v>1046</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="I53" s="4">
         <v>10</v>
@@ -4104,13 +4593,22 @@
         <v>387061</v>
       </c>
       <c r="L53" s="1">
+        <v>48</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" s="1">
         <v>1049</v>
       </c>
-      <c r="M53" t="s">
-        <v>276</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>277</v>
+      <c r="P53" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add talent unlock level
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\nevergiveup\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A579A945-D75F-40DD-94DE-BDEC93B08346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="291">
   <si>
     <t>int</t>
   </si>
@@ -102,6 +98,9 @@
     <t>descCN</t>
   </si>
   <si>
+    <t>unlockLevel</t>
+  </si>
+  <si>
     <t>TalentTreeid</t>
   </si>
   <si>
@@ -153,6 +152,9 @@
     <t>描述备注</t>
   </si>
   <si>
+    <t>解锁当前天赋的玩家等级</t>
+  </si>
+  <si>
     <t>TalentTree_Name_1</t>
   </si>
   <si>
@@ -168,6 +170,9 @@
     <t>12.5|-2</t>
   </si>
   <si>
+    <t>#000000</t>
+  </si>
+  <si>
     <t>TalentTree_Desc_1</t>
   </si>
   <si>
@@ -858,6 +863,9 @@
     <t>1|100||2|100</t>
   </si>
   <si>
+    <t>4.5|4.5</t>
+  </si>
+  <si>
     <t>TalentTree_Desc_47</t>
   </si>
   <si>
@@ -892,21 +900,19 @@
   </si>
   <si>
     <t>在无尽模式下，基地耐久提高{0}</t>
-  </si>
-  <si>
-    <t>4.5|4.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>#000000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -920,35 +926,358 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -956,9 +1285,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -975,21 +1546,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1239,19 +1854,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="22.375" customWidth="1"/>
@@ -1266,7 +1881,7 @@
     <col min="17" max="17" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1318,8 +1933,11 @@
       <c r="Q1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1371,73 +1989,79 @@
       <c r="Q2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" ht="42" customHeight="1" spans="1:18">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="5" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="R3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" ht="42" customHeight="1"/>
+    <row r="5" ht="16.5" spans="1:18">
       <c r="A5" s="1">
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1446,7 +2070,7 @@
         <v>1004</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
@@ -1461,33 +2085,36 @@
         <v>48</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O5" s="1">
         <v>1001</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="16.5" spans="1:18">
       <c r="A6" s="1">
         <v>1002</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1496,7 +2123,7 @@
         <v>1004</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I6" s="2">
         <v>2</v>
@@ -1511,42 +2138,45 @@
         <v>48</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O6" s="1">
         <v>1002</v>
       </c>
       <c r="P6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="16.5" spans="1:18">
       <c r="A7" s="1">
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I7" s="2">
         <v>3</v>
@@ -1561,45 +2191,48 @@
         <v>48</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O7" s="1">
         <v>1003</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="16.5" spans="1:18">
       <c r="A8" s="1">
         <v>1004</v>
       </c>
       <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="I8" s="2">
         <v>3</v>
@@ -1614,33 +2247,36 @@
         <v>48</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O8" s="1">
         <v>1004</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="16.5" spans="1:18">
       <c r="A9" s="1">
         <v>1005</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1652,7 +2288,7 @@
         <v>1010</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -1667,33 +2303,36 @@
         <v>48</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O9" s="1">
         <v>1005</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="16.5" spans="1:18">
       <c r="A10" s="1">
         <v>1006</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1705,7 +2344,7 @@
         <v>1014</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I10" s="2">
         <v>5</v>
@@ -1720,33 +2359,36 @@
         <v>48</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O10" s="1">
         <v>1006</v>
       </c>
       <c r="P10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="16.5" spans="1:18">
       <c r="A11" s="1">
         <v>1007</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -1758,7 +2400,7 @@
         <v>1011</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1773,33 +2415,36 @@
         <v>48</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O11" s="1">
         <v>1007</v>
       </c>
       <c r="P11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" spans="1:18">
       <c r="A12" s="1">
         <v>1008</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1811,7 +2456,7 @@
         <v>1012</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -1826,33 +2471,36 @@
         <v>48</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O12" s="1">
         <v>1008</v>
       </c>
       <c r="P12" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="16.5" spans="1:18">
       <c r="A13" s="1">
         <v>1009</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1864,7 +2512,7 @@
         <v>1013</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I13" s="2">
         <v>2</v>
@@ -1879,33 +2527,36 @@
         <v>48</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O13" s="1">
         <v>1009</v>
       </c>
       <c r="P13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="16.5" spans="1:18">
       <c r="A14" s="1">
         <v>1010</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1917,7 +2568,7 @@
         <v>1014</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I14" s="2">
         <v>2</v>
@@ -1932,33 +2583,36 @@
         <v>48</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O14" s="1">
         <v>1010</v>
       </c>
       <c r="P14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" ht="16.5" spans="1:18">
       <c r="A15" s="1">
         <v>1011</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -1970,7 +2624,7 @@
         <v>1015</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
@@ -1985,33 +2639,36 @@
         <v>48</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O15" s="1">
         <v>1011</v>
       </c>
       <c r="P15" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" ht="16.5" spans="1:18">
       <c r="A16" s="1">
         <v>1012</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2023,7 +2680,7 @@
         <v>1015</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I16" s="2">
         <v>2</v>
@@ -2038,33 +2695,36 @@
         <v>48</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O16" s="1">
         <v>1012</v>
       </c>
       <c r="P16" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" ht="16.5" spans="1:18">
       <c r="A17" s="1">
         <v>1013</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -2076,7 +2736,7 @@
         <v>1015</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I17" s="2">
         <v>2</v>
@@ -2091,45 +2751,48 @@
         <v>48</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O17" s="1">
         <v>1013</v>
       </c>
       <c r="P17" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" ht="16.5" spans="1:18">
       <c r="A18" s="1">
         <v>1014</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G18" s="1">
         <v>1015</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I18" s="2">
         <v>3</v>
@@ -2144,45 +2807,48 @@
         <v>48</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O18" s="1">
         <v>1014</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" ht="16.5" spans="1:18">
       <c r="A19" s="1">
         <v>1015</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I19" s="2">
         <v>4</v>
@@ -2197,33 +2863,36 @@
         <v>48</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O19" s="1">
         <v>1015</v>
       </c>
       <c r="P19" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" ht="16.5" spans="1:18">
       <c r="A20" s="1">
         <v>1016</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -2235,7 +2904,7 @@
         <v>1020</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I20" s="2">
         <v>2</v>
@@ -2250,33 +2919,36 @@
         <v>48</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O20" s="1">
         <v>1016</v>
       </c>
       <c r="P20" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" ht="16.5" spans="1:18">
       <c r="A21" s="1">
         <v>1017</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -2288,7 +2960,7 @@
         <v>1021</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I21" s="2">
         <v>1</v>
@@ -2303,33 +2975,36 @@
         <v>48</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O21" s="1">
         <v>1017</v>
       </c>
       <c r="P21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" ht="16.5" spans="1:18">
       <c r="A22" s="1">
         <v>1018</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -2341,7 +3016,7 @@
         <v>1023</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I22" s="2">
         <v>4</v>
@@ -2356,33 +3031,36 @@
         <v>48</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O22" s="1">
         <v>1018</v>
       </c>
       <c r="P22" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="16.5" spans="1:18">
       <c r="A23" s="1">
         <v>1019</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2394,7 +3072,7 @@
         <v>1023</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I23" s="2">
         <v>4</v>
@@ -2409,33 +3087,36 @@
         <v>48</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O23" s="1">
         <v>1019</v>
       </c>
       <c r="P23" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" ht="16.5" spans="1:18">
       <c r="A24" s="1">
         <v>1020</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -2447,7 +3128,7 @@
         <v>1022</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I24" s="2">
         <v>2</v>
@@ -2462,33 +3143,36 @@
         <v>48</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O24" s="1">
         <v>1020</v>
       </c>
       <c r="P24" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" ht="16.5" spans="1:18">
       <c r="A25" s="1">
         <v>1021</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -2500,7 +3184,7 @@
         <v>1022</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I25" s="2">
         <v>1</v>
@@ -2515,45 +3199,48 @@
         <v>48</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O25" s="1">
         <v>1021</v>
       </c>
       <c r="P25" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="16.5" spans="1:18">
       <c r="A26" s="1">
         <v>1022</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G26" s="1">
         <v>1024</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I26" s="2">
         <v>3</v>
@@ -2568,45 +3255,48 @@
         <v>48</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O26" s="1">
         <v>1022</v>
       </c>
       <c r="P26" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" ht="16.5" spans="1:18">
       <c r="A27" s="1">
         <v>1023</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G27" s="1">
         <v>1024</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I27" s="2">
         <v>3</v>
@@ -2621,45 +3311,48 @@
         <v>48</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O27" s="1">
         <v>1023</v>
       </c>
       <c r="P27" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="16.5" spans="1:18">
       <c r="A28" s="1">
         <v>1024</v>
       </c>
       <c r="B28" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I28" s="2">
         <v>4</v>
@@ -2674,33 +3367,36 @@
         <v>48</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O28" s="1">
         <v>1024</v>
       </c>
       <c r="P28" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="16.5" spans="1:18">
       <c r="A29" s="1">
         <v>1025</v>
       </c>
       <c r="B29" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2712,7 +3408,7 @@
         <v>1028</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I29" s="2">
         <v>3</v>
@@ -2727,33 +3423,36 @@
         <v>48</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O29" s="1">
         <v>1025</v>
       </c>
       <c r="P29" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="16.5" spans="1:18">
       <c r="A30" s="1">
         <v>1026</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2765,7 +3464,7 @@
         <v>1028</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I30" s="2">
         <v>3</v>
@@ -2780,33 +3479,36 @@
         <v>48</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O30" s="1">
         <v>1026</v>
       </c>
       <c r="P30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="16.5" spans="1:18">
       <c r="A31" s="1">
         <v>1027</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2815,10 +3517,10 @@
         <v>1024</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I31" s="2">
         <v>3</v>
@@ -2833,45 +3535,48 @@
         <v>48</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O31" s="1">
         <v>1027</v>
       </c>
       <c r="P31" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="16.5" spans="1:18">
       <c r="A32" s="1">
         <v>1028</v>
       </c>
       <c r="B32" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I32" s="2">
         <v>3</v>
@@ -2886,33 +3591,36 @@
         <v>48</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N32" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O32" s="1">
         <v>1028</v>
       </c>
       <c r="P32" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="16.5" spans="1:18">
       <c r="A33" s="1">
         <v>1029</v>
       </c>
       <c r="B33" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -2924,7 +3632,7 @@
         <v>1034</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I33" s="2">
         <v>2</v>
@@ -2939,33 +3647,36 @@
         <v>48</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O33" s="1">
         <v>1029</v>
       </c>
       <c r="P33" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="16.5" spans="1:18">
       <c r="A34" s="1">
         <v>1030</v>
       </c>
       <c r="B34" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2977,7 +3688,7 @@
         <v>1038</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
@@ -2992,33 +3703,36 @@
         <v>48</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O34" s="1">
         <v>1030</v>
       </c>
       <c r="P34" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q34" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="16.5" spans="1:18">
       <c r="A35" s="1">
         <v>1031</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -3030,7 +3744,7 @@
         <v>1035</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I35" s="2">
         <v>2</v>
@@ -3045,33 +3759,36 @@
         <v>48</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O35" s="1">
         <v>1031</v>
       </c>
       <c r="P35" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="16.5" spans="1:18">
       <c r="A36" s="1">
         <v>1032</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -3083,7 +3800,7 @@
         <v>1036</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I36" s="2">
         <v>2</v>
@@ -3098,33 +3815,36 @@
         <v>48</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O36" s="1">
         <v>1032</v>
       </c>
       <c r="P36" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="16.5" spans="1:18">
       <c r="A37" s="1">
         <v>1033</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -3136,7 +3856,7 @@
         <v>1037</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I37" s="2">
         <v>2</v>
@@ -3151,33 +3871,36 @@
         <v>48</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O37" s="1">
         <v>1033</v>
       </c>
       <c r="P37" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="16.5" spans="1:18">
       <c r="A38" s="1">
         <v>1034</v>
       </c>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -3189,7 +3912,7 @@
         <v>1038</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I38" s="2">
         <v>2</v>
@@ -3204,33 +3927,36 @@
         <v>48</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O38" s="1">
         <v>1034</v>
       </c>
       <c r="P38" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="16.5" spans="1:18">
       <c r="A39" s="1">
         <v>1035</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -3242,7 +3968,7 @@
         <v>1039</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I39" s="2">
         <v>2</v>
@@ -3257,33 +3983,36 @@
         <v>48</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O39" s="1">
         <v>1035</v>
       </c>
       <c r="P39" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="16.5" spans="1:18">
       <c r="A40" s="1">
         <v>1036</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -3295,7 +4024,7 @@
         <v>1039</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I40" s="2">
         <v>2</v>
@@ -3310,33 +4039,36 @@
         <v>48</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O40" s="1">
         <v>1036</v>
       </c>
       <c r="P40" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="16.5" spans="1:18">
       <c r="A41" s="1">
         <v>1037</v>
       </c>
       <c r="B41" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -3348,7 +4080,7 @@
         <v>1039</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I41" s="2">
         <v>2</v>
@@ -3363,45 +4095,48 @@
         <v>48</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O41" s="1">
         <v>1037</v>
       </c>
       <c r="P41" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" ht="16.5" spans="1:18">
       <c r="A42" s="1">
         <v>1038</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G42" s="1">
         <v>1039</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I42" s="2">
         <v>3</v>
@@ -3416,45 +4151,48 @@
         <v>48</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N42" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O42" s="1">
         <v>1038</v>
       </c>
       <c r="P42" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" ht="16.5" spans="1:18">
       <c r="A43" s="1">
         <v>1039</v>
       </c>
       <c r="B43" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I43" s="2">
         <v>4</v>
@@ -3469,33 +4207,36 @@
         <v>48</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N43" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O43" s="1">
         <v>1039</v>
       </c>
       <c r="P43" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" ht="16.5" spans="1:18">
       <c r="A44" s="1">
         <v>1040</v>
       </c>
       <c r="B44" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -3507,7 +4248,7 @@
         <v>1044</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I44" s="2">
         <v>2</v>
@@ -3522,33 +4263,36 @@
         <v>48</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O44" s="1">
         <v>1040</v>
       </c>
       <c r="P44" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" ht="16.5" spans="1:18">
       <c r="A45" s="1">
         <v>1041</v>
       </c>
       <c r="B45" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -3560,7 +4304,7 @@
         <v>1045</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I45" s="2">
         <v>1</v>
@@ -3575,33 +4319,36 @@
         <v>48</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N45" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O45" s="1">
         <v>1041</v>
       </c>
       <c r="P45" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="16.5" spans="1:18">
       <c r="A46" s="1">
         <v>1042</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -3613,7 +4360,7 @@
         <v>1046</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I46" s="2">
         <v>4</v>
@@ -3628,33 +4375,36 @@
         <v>48</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N46" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O46" s="1">
         <v>1042</v>
       </c>
       <c r="P46" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" ht="16.5" spans="1:18">
       <c r="A47" s="1">
         <v>1043</v>
       </c>
       <c r="B47" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -3666,7 +4416,7 @@
         <v>1046</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I47" s="2">
         <v>4</v>
@@ -3681,33 +4431,36 @@
         <v>48</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O47" s="1">
         <v>1043</v>
       </c>
       <c r="P47" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" ht="16.5" spans="1:18">
       <c r="A48" s="1">
         <v>1044</v>
       </c>
       <c r="B48" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -3719,7 +4472,7 @@
         <v>1046</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I48" s="2">
         <v>2</v>
@@ -3734,33 +4487,36 @@
         <v>48</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N48" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O48" s="1">
         <v>1044</v>
       </c>
       <c r="P48" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" ht="16.5" spans="1:18">
       <c r="A49" s="1">
         <v>1045</v>
       </c>
       <c r="B49" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -3772,7 +4528,7 @@
         <v>1046</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I49" s="2">
         <v>1</v>
@@ -3787,45 +4543,48 @@
         <v>48</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N49" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O49" s="1">
         <v>1045</v>
       </c>
       <c r="P49" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" ht="16.5" spans="1:18">
       <c r="A50" s="1">
         <v>1046</v>
       </c>
       <c r="B50" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I50" s="2">
         <v>4</v>
@@ -3840,33 +4599,36 @@
         <v>48</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>288</v>
+        <v>46</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O50" s="1">
         <v>1046</v>
       </c>
       <c r="P50" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" ht="16.5" spans="1:18">
       <c r="A51" s="1">
         <v>1047</v>
       </c>
       <c r="B51" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -3875,7 +4637,7 @@
         <v>1046</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I51" s="2">
         <v>10</v>
@@ -3889,34 +4651,37 @@
       <c r="L51" s="1">
         <v>72</v>
       </c>
-      <c r="M51" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="N51" s="4" t="s">
-        <v>288</v>
+      <c r="M51" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O51" s="1">
         <v>1047</v>
       </c>
       <c r="P51" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" ht="16.5" spans="1:18">
       <c r="A52" s="1">
         <v>1048</v>
       </c>
       <c r="B52" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -3925,7 +4690,7 @@
         <v>1046</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I52" s="2">
         <v>10</v>
@@ -3939,34 +4704,37 @@
       <c r="L52" s="1">
         <v>72</v>
       </c>
-      <c r="M52" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="N52" s="4" t="s">
-        <v>288</v>
+      <c r="M52" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O52" s="1">
         <v>1048</v>
       </c>
       <c r="P52" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" ht="16.5" spans="1:18">
       <c r="A53" s="1">
         <v>1049</v>
       </c>
       <c r="B53" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -3975,7 +4743,7 @@
         <v>1046</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I53" s="2">
         <v>10</v>
@@ -3989,25 +4757,28 @@
       <c r="L53" s="1">
         <v>72</v>
       </c>
-      <c r="M53" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="N53" s="4" t="s">
-        <v>288</v>
+      <c r="M53" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="O53" s="1">
         <v>1049</v>
       </c>
       <c r="P53" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update eleven UI
更新11修改的UI
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\nevergiveup\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D04600B-29B4-4D8E-B8BE-CAD919DB3A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE62CC8-BBE6-4DD9-A2EF-7425582B02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4041,7 +4041,7 @@
         <v>387060</v>
       </c>
       <c r="L51" s="1">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="M51" s="3" t="s">
         <v>272</v>
@@ -4094,7 +4094,7 @@
         <v>387059</v>
       </c>
       <c r="L52" s="1">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="M52" s="3" t="s">
         <v>272</v>
@@ -4147,7 +4147,7 @@
         <v>387061</v>
       </c>
       <c r="L53" s="1">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="M53" s="3" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
feat: update UI and language
调整UI优化和多语言
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE62CC8-BBE6-4DD9-A2EF-7425582B02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC23574-8EB4-467C-B656-01D7E6458B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,9 +849,6 @@
     <t>talentItemCanvas_47</t>
   </si>
   <si>
-    <t>4.5|4.5</t>
-  </si>
-  <si>
     <t>TalentTree_Desc_47</t>
   </si>
   <si>
@@ -904,6 +901,10 @@
   </si>
   <si>
     <t>1|200||2|200</t>
+  </si>
+  <si>
+    <t>0|-4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1255,7 +1256,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1462,7 +1463,7 @@
         <v>1004</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I5" s="2">
         <v>2</v>
@@ -1515,7 +1516,7 @@
         <v>1004</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I6" s="2">
         <v>2</v>
@@ -1568,7 +1569,7 @@
         <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I7" s="2">
         <v>3</v>
@@ -1624,7 +1625,7 @@
         <v>64</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I8" s="2">
         <v>3</v>
@@ -1680,7 +1681,7 @@
         <v>1010</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -1736,7 +1737,7 @@
         <v>1014</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I10" s="2">
         <v>5</v>
@@ -1792,7 +1793,7 @@
         <v>1011</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
@@ -1848,7 +1849,7 @@
         <v>1012</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -1904,7 +1905,7 @@
         <v>1013</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I13" s="2">
         <v>2</v>
@@ -1960,7 +1961,7 @@
         <v>1014</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I14" s="2">
         <v>2</v>
@@ -2016,7 +2017,7 @@
         <v>1015</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
@@ -2072,7 +2073,7 @@
         <v>1015</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I16" s="2">
         <v>2</v>
@@ -2128,7 +2129,7 @@
         <v>1015</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I17" s="2">
         <v>2</v>
@@ -2184,7 +2185,7 @@
         <v>1015</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I18" s="2">
         <v>3</v>
@@ -2240,7 +2241,7 @@
         <v>122</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I19" s="2">
         <v>4</v>
@@ -2296,7 +2297,7 @@
         <v>1020</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I20" s="2">
         <v>2</v>
@@ -2352,7 +2353,7 @@
         <v>1021</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I21" s="2">
         <v>1</v>
@@ -2408,7 +2409,7 @@
         <v>1023</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I22" s="2">
         <v>4</v>
@@ -2464,7 +2465,7 @@
         <v>1023</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I23" s="2">
         <v>4</v>
@@ -2520,7 +2521,7 @@
         <v>1022</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I24" s="2">
         <v>2</v>
@@ -2576,7 +2577,7 @@
         <v>1022</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I25" s="2">
         <v>1</v>
@@ -2632,7 +2633,7 @@
         <v>1024</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I26" s="2">
         <v>3</v>
@@ -2688,7 +2689,7 @@
         <v>1024</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I27" s="2">
         <v>3</v>
@@ -2744,7 +2745,7 @@
         <v>171</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I28" s="2">
         <v>4</v>
@@ -2800,7 +2801,7 @@
         <v>1028</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I29" s="2">
         <v>3</v>
@@ -2856,7 +2857,7 @@
         <v>1028</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I30" s="2">
         <v>3</v>
@@ -2912,7 +2913,7 @@
         <v>184</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I31" s="2">
         <v>3</v>
@@ -2968,7 +2969,7 @@
         <v>190</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I32" s="2">
         <v>3</v>
@@ -3024,7 +3025,7 @@
         <v>1034</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I33" s="2">
         <v>2</v>
@@ -3080,7 +3081,7 @@
         <v>1038</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
@@ -3136,7 +3137,7 @@
         <v>1035</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I35" s="2">
         <v>2</v>
@@ -3192,7 +3193,7 @@
         <v>1036</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I36" s="2">
         <v>2</v>
@@ -3248,7 +3249,7 @@
         <v>1037</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I37" s="2">
         <v>2</v>
@@ -3304,7 +3305,7 @@
         <v>1038</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I38" s="2">
         <v>2</v>
@@ -3360,7 +3361,7 @@
         <v>1039</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I39" s="2">
         <v>2</v>
@@ -3416,7 +3417,7 @@
         <v>1039</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I40" s="2">
         <v>2</v>
@@ -3472,7 +3473,7 @@
         <v>1039</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I41" s="2">
         <v>2</v>
@@ -3528,7 +3529,7 @@
         <v>1039</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I42" s="2">
         <v>3</v>
@@ -3584,7 +3585,7 @@
         <v>237</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I43" s="2">
         <v>4</v>
@@ -3640,7 +3641,7 @@
         <v>1044</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I44" s="2">
         <v>2</v>
@@ -3696,7 +3697,7 @@
         <v>1045</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I45" s="2">
         <v>1</v>
@@ -3752,7 +3753,7 @@
         <v>1046</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I46" s="2">
         <v>4</v>
@@ -3808,7 +3809,7 @@
         <v>1046</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I47" s="2">
         <v>4</v>
@@ -3864,7 +3865,7 @@
         <v>1046</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I48" s="2">
         <v>2</v>
@@ -3920,7 +3921,7 @@
         <v>1046</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I49" s="2">
         <v>1</v>
@@ -3976,7 +3977,7 @@
         <v>267</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I50" s="2">
         <v>4</v>
@@ -4029,7 +4030,7 @@
         <v>1046</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I51" s="2">
         <v>10</v>
@@ -4044,7 +4045,7 @@
         <v>80</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="N51" s="3" t="s">
         <v>46</v>
@@ -4053,10 +4054,10 @@
         <v>1047</v>
       </c>
       <c r="P51" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q51" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -4067,13 +4068,13 @@
         <v>1048</v>
       </c>
       <c r="B52" t="s">
+        <v>274</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -4082,7 +4083,7 @@
         <v>1046</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I52" s="2">
         <v>10</v>
@@ -4097,7 +4098,7 @@
         <v>80</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="N52" s="3" t="s">
         <v>46</v>
@@ -4106,10 +4107,10 @@
         <v>1048</v>
       </c>
       <c r="P52" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q52" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="R52">
         <v>0</v>
@@ -4120,13 +4121,13 @@
         <v>1049</v>
       </c>
       <c r="B53" t="s">
+        <v>279</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="E53" s="1">
         <v>2</v>
@@ -4135,7 +4136,7 @@
         <v>1046</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I53" s="2">
         <v>10</v>
@@ -4150,7 +4151,7 @@
         <v>80</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="N53" s="3" t="s">
         <v>46</v>
@@ -4159,10 +4160,10 @@
         <v>1049</v>
       </c>
       <c r="P53" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q53" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="Q53" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="R53">
         <v>0</v>

</xml_diff>

<commit_message>
feat: update Stage TalentTree
更新关卡通关奖励和天赋树解锁等级
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/TalentTree_天赋树表.xlsx
+++ b/nevergiveup/Excel/TalentTree_天赋树表.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6070DABF-2D22-4BE2-B7B4-61447240C913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E86B9-F3B4-44CA-B91D-FF869F8065D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="Y49" sqref="Y49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3217,7 +3217,7 @@
         <v>138</v>
       </c>
       <c r="W28">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="16.5" x14ac:dyDescent="0.35">
@@ -4282,7 +4282,7 @@
         <v>138</v>
       </c>
       <c r="W43">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="16.5" x14ac:dyDescent="0.35">
@@ -4779,7 +4779,7 @@
         <v>138</v>
       </c>
       <c r="W50">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="16.5" x14ac:dyDescent="0.35">

</xml_diff>